<commit_message>
Add completed REV3 BOM
</commit_message>
<xml_diff>
--- a/BOMs/REV3/BOM-full.xlsx
+++ b/BOMs/REV3/BOM-full.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\AoM\IoT-Bit\AoM-IoT-Bit\BOMs\REV3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC79AB1D-6D18-41C1-B826-580CAB91C9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1D0C62-28B2-4437-86DE-D9D87F1FAA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="REV3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
   <si>
     <t>Name/Desc</t>
   </si>
@@ -42,15 +42,6 @@
     <t>Vendor Link</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Price </t>
-  </si>
-  <si>
-    <t>Num/Units</t>
-  </si>
-  <si>
-    <t>Total Haul Price</t>
-  </si>
-  <si>
     <t>Arduino MKR WiFi 1010</t>
   </si>
   <si>
@@ -166,6 +157,87 @@
   </si>
   <si>
     <t>https://www.amazon.com/dp/B0876H387X/</t>
+  </si>
+  <si>
+    <t>ABX00023</t>
+  </si>
+  <si>
+    <t>https://store-usa.arduino.cc/products/arduino-mkr-wifi-1010</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/</t>
+  </si>
+  <si>
+    <t>650-0071</t>
+  </si>
+  <si>
+    <t>B02B-PASK(LF)(SN)</t>
+  </si>
+  <si>
+    <t>PAP-02V-S</t>
+  </si>
+  <si>
+    <t>PAP-03V-S</t>
+  </si>
+  <si>
+    <t>B03B-PASK-1(LF)(SN)</t>
+  </si>
+  <si>
+    <t>SPHD-002T-P0.5</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/779</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/777</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3347</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2179</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3221</t>
+  </si>
+  <si>
+    <t>OMEGA</t>
+  </si>
+  <si>
+    <t>1569-26-1-0500-003-1-TS</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cnc-tech/1569-26-1-0500-003-1-TS/15853701</t>
+  </si>
+  <si>
+    <t>1569-26-1-0500-004-1-TS</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cnc-tech/1569-26-1-0500-004-1-TS/15853684</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cnc-tech/1569-26-1-0500-001-1-TS/15853661</t>
+  </si>
+  <si>
+    <t>1569-26-1-0500-001-1-TS</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B02B-PASK-1-LF-SN/926738</t>
+  </si>
+  <si>
+    <t>https://sphero.com/products/wire-bit</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/PAP-02V-S/759974</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B03B-PASK-1-LF-SN/926739</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/PAP-03V-S/759975</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/SPHD-002T-P0-5/608754</t>
   </si>
 </sst>
 </file>
@@ -176,7 +248,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,17 +264,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -252,25 +331,34 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -553,29 +641,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.44140625" customWidth="1"/>
     <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="6"/>
-    <col min="6" max="6" width="42.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="84.44140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -587,260 +674,461 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="D2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="1">
+        <v>14</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D12" s="1">
+        <v>777</v>
+      </c>
+      <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="F12" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1">
+        <v>779</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3347</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2179</v>
+      </c>
+      <c r="E15" s="1">
+        <v>4</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3221</v>
+      </c>
+      <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="6">
-        <v>4</v>
-      </c>
       <c r="F16" s="7" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="6">
-        <v>4</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="1">
+        <v>6</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="1">
+        <v>6</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="1">
+        <v>6</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="1">
+        <v>6</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="6">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="1">
         <v>1</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="6">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="1">
         <v>1</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F17" r:id="rId1" xr:uid="{395CA26B-C372-4BCE-B71B-6878E6A827BB}"/>
-    <hyperlink ref="F16" r:id="rId2" xr:uid="{4246AF7A-FBFC-40E7-A1DA-37350360E38B}"/>
+    <hyperlink ref="F18" r:id="rId1" xr:uid="{395CA26B-C372-4BCE-B71B-6878E6A827BB}"/>
+    <hyperlink ref="F17" r:id="rId2" xr:uid="{4246AF7A-FBFC-40E7-A1DA-37350360E38B}"/>
     <hyperlink ref="F5" r:id="rId3" xr:uid="{526DDF5D-738D-4C21-8AF7-AE0D3475A2B8}"/>
     <hyperlink ref="F6" r:id="rId4" xr:uid="{551CAEA5-0508-417C-BF9C-46502D6657E4}"/>
     <hyperlink ref="F25" r:id="rId5" xr:uid="{42298739-9446-4191-BA19-43DA75F5D409}"/>
+    <hyperlink ref="F2" r:id="rId6" xr:uid="{A0853A55-39FE-4A61-B733-541D7BD0DAA5}"/>
+    <hyperlink ref="F3" r:id="rId7" xr:uid="{9B7CEB9B-C71E-4892-9CE2-4CAAF5C9F6FD}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{2EC75BBB-A27C-4565-BF63-3611C12859B5}"/>
+    <hyperlink ref="F13" r:id="rId9" xr:uid="{427D79DB-CA97-4DD4-B0B3-B3707BE05116}"/>
+    <hyperlink ref="F14" r:id="rId10" xr:uid="{CD841108-D1A4-45AA-AD4E-52F415CE3ABA}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{AFF8580F-8C4E-42AA-9559-A2E1B895ED58}"/>
+    <hyperlink ref="F16" r:id="rId12" xr:uid="{076A1A47-4427-40E0-A484-5B42659EF6B5}"/>
+    <hyperlink ref="F21" r:id="rId13" xr:uid="{A74E746E-66F3-4868-8B2A-C6FED812F19A}"/>
+    <hyperlink ref="F19" r:id="rId14" xr:uid="{9EA4F340-8996-4D75-BFE3-CCDE8AEFE285}"/>
+    <hyperlink ref="F20" r:id="rId15" xr:uid="{702F0467-C113-45A6-A0BE-198E545D2585}"/>
+    <hyperlink ref="F7" r:id="rId16" xr:uid="{E0813DEE-78B5-4C3C-93D9-76AC144775D4}"/>
+    <hyperlink ref="F8" r:id="rId17" xr:uid="{D499380E-1374-4D4B-BA97-3F0D6B8B0810}"/>
+    <hyperlink ref="F9" r:id="rId18" xr:uid="{0732D53C-2256-4E4D-8624-C189E90570BF}"/>
+    <hyperlink ref="F10" r:id="rId19" xr:uid="{34CA46BC-F410-47C8-9B2F-EACD022CE32B}"/>
+    <hyperlink ref="F11" r:id="rId20" xr:uid="{00F95A36-C49F-4BEC-9979-06FFCFA5418D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>